<commit_message>
Correcciones global.r Definicion de ui y server Carga carpeta data
</commit_message>
<xml_diff>
--- a/datos_crudos/RS-ING-09 PLANILLA REGISTRO P.E.10-03-16.xlsx
+++ b/datos_crudos/RS-ING-09 PLANILLA REGISTRO P.E.10-03-16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria en Ciencias de Datos\Analisis inteligente de datos\TP Final\TP Final AID Del Bo\trabajo-final-tomasdelbo\datos_crudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE74254-97CA-408E-ACF7-8C6014386C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA610CD-569E-4372-AEAF-DF1A0B722DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="1531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="1532">
   <si>
     <t>CODIFICACION DE EQUIPOS EN PEDIDOS ESPECIALES</t>
   </si>
@@ -4841,6 +4841,9 @@
   </si>
   <si>
     <t>Se necesita cotizar equipo tipo ciabattera para realizar los siguientes productos: 1- Pizza rectangular 18x38 y 18x18 de 4 o 5 mm de espesor. 2-Ciabatta 2 tamaños uno corto y uno más largo tipo baguette rústica Pizza redonda D350 y D240mm. (Aceptarían bajar a D305 para que entren dos unidades en el ancho). Las pizzas rectangulares de 18x34 en el orden de 24 piezas por minuto. Lo cual está dentro del rango de la velocidad de la máquina. El espesor de la masa de 4-5 mm si o si debe ser con calibrador multi rolo se debe cotizar especial. La transferencia a el transportador del horno requiere un estibador tipo puente que tampoco sería el estándar del equipo.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -5054,7 +5057,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5101,12 +5104,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF33CC"/>
         <bgColor rgb="FFFF00FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -5545,7 +5542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5821,9 +5818,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
@@ -5852,6 +5846,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5866,21 +5875,6 @@
     </xf>
     <xf numFmtId="165" fontId="18" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6339,12 +6333,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7326,7 +7320,7 @@
   <dimension ref="A1:E416"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
@@ -7339,18 +7333,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
     </row>
     <row r="2" spans="1:5" s="38" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="133" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
       <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:5" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12024,14 +12018,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="134" t="s">
         <v>566</v>
       </c>
-      <c r="B1" s="135"/>
+      <c r="B1" s="134"/>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="135"/>
-      <c r="B2" s="135"/>
+      <c r="A2" s="134"/>
+      <c r="B2" s="134"/>
     </row>
     <row r="3" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
@@ -17987,10 +17981,10 @@
   </sheetPr>
   <dimension ref="A1:X107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="71" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -18019,103 +18013,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="90" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="141"/>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="142" t="s">
+      <c r="A1" s="135"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="136" t="s">
         <v>1314</v>
       </c>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142"/>
-      <c r="M1" s="142"/>
-      <c r="N1" s="142"/>
-      <c r="O1" s="142"/>
-      <c r="P1" s="142"/>
-      <c r="Q1" s="142"/>
-      <c r="R1" s="142"/>
-      <c r="S1" s="142"/>
-      <c r="T1" s="142"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136"/>
+      <c r="S1" s="136"/>
+      <c r="T1" s="136"/>
     </row>
     <row r="2" spans="1:24" s="91" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="141"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="143" t="s">
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="137" t="s">
         <v>1315</v>
       </c>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="143"/>
-      <c r="S2" s="143"/>
-      <c r="T2" s="143"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="137"/>
+      <c r="N2" s="137"/>
+      <c r="O2" s="137"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="137"/>
+      <c r="S2" s="137"/>
+      <c r="T2" s="137"/>
     </row>
     <row r="3" spans="1:24" s="90" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="138" t="s">
         <v>1316</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="145" t="s">
+      <c r="B3" s="138"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="139" t="s">
         <v>1317</v>
       </c>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="145"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="145"/>
-      <c r="O3" s="145"/>
-      <c r="P3" s="145"/>
-      <c r="Q3" s="145"/>
-      <c r="R3" s="145"/>
-      <c r="S3" s="145"/>
-      <c r="T3" s="145"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
+      <c r="T3" s="139"/>
     </row>
     <row r="4" spans="1:24" s="93" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="92" t="s">
         <v>1318</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="140" t="s">
         <v>1319</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="137"/>
-      <c r="K4" s="137"/>
-      <c r="L4" s="137"/>
-      <c r="M4" s="137"/>
-      <c r="N4" s="137"/>
-      <c r="O4" s="137"/>
-      <c r="P4" s="138" t="s">
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="141"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="141"/>
+      <c r="M4" s="141"/>
+      <c r="N4" s="141"/>
+      <c r="O4" s="141"/>
+      <c r="P4" s="142" t="s">
         <v>1320</v>
       </c>
-      <c r="Q4" s="138"/>
+      <c r="Q4" s="142"/>
     </row>
     <row r="5" spans="1:24" s="94" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="94" t="s">
@@ -18193,26 +18187,26 @@
     </row>
     <row r="6" spans="1:24" s="94" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="106"/>
-      <c r="B6" s="139"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="139"/>
-      <c r="M6" s="139"/>
-      <c r="N6" s="139"/>
-      <c r="O6" s="139"/>
-      <c r="P6" s="139"/>
-      <c r="Q6" s="139"/>
-      <c r="R6" s="140" t="s">
+      <c r="B6" s="143"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="143"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
+      <c r="R6" s="144" t="s">
         <v>1343</v>
       </c>
-      <c r="S6" s="140"/>
+      <c r="S6" s="144"/>
       <c r="T6" s="107" t="s">
         <v>1344</v>
       </c>
@@ -18242,9 +18236,12 @@
       <c r="E7" s="84">
         <v>45266</v>
       </c>
-      <c r="G7" s="85" t="str">
+      <c r="F7" s="84">
+        <v>45266</v>
+      </c>
+      <c r="G7" s="85">
         <f t="shared" ref="G7:G25" si="0">IF(F7&lt;&gt;"",NETWORKDAYS(E7,F7),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M7" s="83">
         <v>515</v>
@@ -18278,9 +18275,12 @@
       <c r="E8" s="84">
         <v>45268</v>
       </c>
-      <c r="G8" s="85" t="str">
+      <c r="F8" s="84">
+        <v>45268</v>
+      </c>
+      <c r="G8" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M8" s="83">
         <v>317</v>
@@ -18302,15 +18302,18 @@
       <c r="C9" s="83">
         <v>707</v>
       </c>
-      <c r="D9" s="130" t="s">
+      <c r="D9" s="129" t="s">
         <v>1386</v>
       </c>
       <c r="E9" s="84">
         <v>45268</v>
       </c>
-      <c r="G9" s="85" t="str">
+      <c r="F9" s="84">
+        <v>45268</v>
+      </c>
+      <c r="G9" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M9" s="83">
         <v>152</v>
@@ -18338,9 +18341,12 @@
       <c r="E10" s="84">
         <v>45264</v>
       </c>
-      <c r="G10" s="85" t="str">
+      <c r="F10" s="84">
+        <v>45264</v>
+      </c>
+      <c r="G10" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M10" s="83">
         <v>490</v>
@@ -18368,9 +18374,12 @@
       <c r="E11" s="84">
         <v>45266</v>
       </c>
-      <c r="G11" s="85" t="str">
+      <c r="F11" s="84">
+        <v>45266</v>
+      </c>
+      <c r="G11" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M11" s="83">
         <v>481</v>
@@ -18392,9 +18401,17 @@
       <c r="C12" s="83">
         <v>710</v>
       </c>
-      <c r="G12" s="85" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D12" s="83" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E12" s="84" t="s">
+        <v>1531</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>1531</v>
+      </c>
+      <c r="G12" s="85" t="s">
+        <v>1531</v>
       </c>
       <c r="M12" s="83">
         <v>515</v>
@@ -18422,9 +18439,12 @@
       <c r="E13" s="84">
         <v>45308</v>
       </c>
-      <c r="G13" s="85" t="str">
+      <c r="F13" s="84">
+        <v>45308</v>
+      </c>
+      <c r="G13" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M13" s="83">
         <v>552</v>
@@ -18452,9 +18472,12 @@
       <c r="E14" s="84">
         <v>45315</v>
       </c>
-      <c r="G14" s="85" t="str">
+      <c r="F14" s="84">
+        <v>45315</v>
+      </c>
+      <c r="G14" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M14" s="83">
         <v>543</v>
@@ -18482,9 +18505,12 @@
       <c r="E15" s="84">
         <v>45323</v>
       </c>
-      <c r="G15" s="85" t="str">
+      <c r="F15" s="84">
+        <v>45323</v>
+      </c>
+      <c r="G15" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M15" s="83">
         <v>505</v>
@@ -18506,9 +18532,12 @@
       <c r="E16" s="84">
         <v>38025</v>
       </c>
-      <c r="G16" s="85" t="str">
+      <c r="F16" s="84">
+        <v>38025</v>
+      </c>
+      <c r="G16" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M16" s="83">
         <v>555</v>
@@ -18536,9 +18565,15 @@
       <c r="D17" s="83" t="s">
         <v>1297</v>
       </c>
-      <c r="G17" s="85" t="str">
+      <c r="E17" s="84">
+        <v>38025</v>
+      </c>
+      <c r="F17" s="84">
+        <v>38025</v>
+      </c>
+      <c r="G17" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M17" s="83">
         <v>490</v>
@@ -18566,9 +18601,12 @@
       <c r="E18" s="84">
         <v>44972</v>
       </c>
-      <c r="G18" s="85" t="str">
+      <c r="F18" s="84">
+        <v>44972</v>
+      </c>
+      <c r="G18" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M18" s="83">
         <v>559</v>
@@ -18596,9 +18634,12 @@
       <c r="E19" s="84">
         <v>45342</v>
       </c>
-      <c r="G19" s="85" t="str">
+      <c r="F19" s="84">
+        <v>45342</v>
+      </c>
+      <c r="G19" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M19" s="83">
         <v>481</v>
@@ -18626,9 +18667,12 @@
       <c r="E20" s="84">
         <v>45348</v>
       </c>
-      <c r="G20" s="85" t="str">
+      <c r="F20" s="84">
+        <v>45348</v>
+      </c>
+      <c r="G20" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M20" s="83">
         <v>337</v>
@@ -18656,9 +18700,12 @@
       <c r="E21" s="84">
         <v>45356</v>
       </c>
-      <c r="G21" s="85" t="str">
+      <c r="F21" s="84">
+        <v>45356</v>
+      </c>
+      <c r="G21" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M21" s="83">
         <v>533</v>
@@ -18686,9 +18733,12 @@
       <c r="E22" s="84">
         <v>45363</v>
       </c>
-      <c r="G22" s="85" t="str">
+      <c r="F22" s="84">
+        <v>45363</v>
+      </c>
+      <c r="G22" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M22" s="83">
         <v>560</v>
@@ -18716,9 +18766,12 @@
       <c r="E23" s="84">
         <v>45356</v>
       </c>
-      <c r="G23" s="85" t="str">
+      <c r="F23" s="84">
+        <v>45356</v>
+      </c>
+      <c r="G23" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M23" s="83">
         <v>146</v>
@@ -18746,9 +18799,12 @@
       <c r="E24" s="84">
         <v>45377</v>
       </c>
-      <c r="G24" s="85" t="str">
+      <c r="F24" s="84">
+        <v>45377</v>
+      </c>
+      <c r="G24" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N24" s="83" t="s">
         <v>1354</v>
@@ -18773,9 +18829,12 @@
       <c r="E25" s="84">
         <v>45379</v>
       </c>
-      <c r="G25" s="85" t="str">
+      <c r="F25" s="84">
+        <v>45379</v>
+      </c>
+      <c r="G25" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M25" s="83">
         <v>146</v>
@@ -18803,9 +18862,12 @@
       <c r="E26" s="84">
         <v>45392</v>
       </c>
-      <c r="G26" s="85" t="str">
+      <c r="F26" s="84">
+        <v>45392</v>
+      </c>
+      <c r="G26" s="85">
         <f t="shared" ref="G26:G31" si="1">IF(F25&lt;&gt;"",NETWORKDAYS(E25,F25),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M26" s="83">
         <v>554</v>
@@ -18833,9 +18895,12 @@
       <c r="E27" s="84">
         <v>45392</v>
       </c>
-      <c r="G27" s="85" t="str">
+      <c r="F27" s="84">
+        <v>45392</v>
+      </c>
+      <c r="G27" s="85">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M27" s="83">
         <v>525</v>
@@ -18863,9 +18928,12 @@
       <c r="E28" s="84">
         <v>45394</v>
       </c>
-      <c r="G28" s="85" t="str">
+      <c r="F28" s="84">
+        <v>45394</v>
+      </c>
+      <c r="G28" s="85">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M28" s="83">
         <v>438</v>
@@ -18896,9 +18964,12 @@
       <c r="E29" s="84">
         <v>45398</v>
       </c>
-      <c r="G29" s="85" t="str">
+      <c r="F29" s="84">
+        <v>45398</v>
+      </c>
+      <c r="G29" s="85">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M29" s="83">
         <v>448</v>
@@ -18926,9 +18997,12 @@
       <c r="E30" s="84">
         <v>45394</v>
       </c>
-      <c r="G30" s="85" t="str">
+      <c r="F30" s="84">
+        <v>45394</v>
+      </c>
+      <c r="G30" s="85">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M30" s="83">
         <v>490</v>
@@ -18956,9 +19030,12 @@
       <c r="E31" s="84">
         <v>45411</v>
       </c>
-      <c r="G31" s="85" t="str">
+      <c r="F31" s="84">
+        <v>45411</v>
+      </c>
+      <c r="G31" s="85">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="M31" s="83">
         <v>541</v>
@@ -18986,6 +19063,9 @@
       <c r="E32" s="84">
         <v>45412</v>
       </c>
+      <c r="F32" s="84">
+        <v>45412</v>
+      </c>
       <c r="M32" s="83">
         <v>542</v>
       </c>
@@ -19015,6 +19095,9 @@
       <c r="E33" s="84">
         <v>45425</v>
       </c>
+      <c r="F33" s="84">
+        <v>45425</v>
+      </c>
       <c r="M33" s="83">
         <v>459</v>
       </c>
@@ -19041,6 +19124,9 @@
       <c r="E34" s="84">
         <v>45433</v>
       </c>
+      <c r="F34" s="84">
+        <v>45433</v>
+      </c>
       <c r="M34" s="83">
         <v>441</v>
       </c>
@@ -19070,6 +19156,9 @@
       <c r="E35" s="84">
         <v>45443</v>
       </c>
+      <c r="F35" s="84">
+        <v>45443</v>
+      </c>
       <c r="M35" s="83">
         <v>533</v>
       </c>
@@ -19093,6 +19182,9 @@
       <c r="E36" s="84">
         <v>45456</v>
       </c>
+      <c r="F36" s="84">
+        <v>45456</v>
+      </c>
       <c r="M36" s="83">
         <v>317</v>
       </c>
@@ -19119,6 +19211,9 @@
       <c r="E37" s="84">
         <v>45467</v>
       </c>
+      <c r="F37" s="84">
+        <v>45467</v>
+      </c>
       <c r="M37" s="83">
         <v>513</v>
       </c>
@@ -19148,6 +19243,9 @@
       <c r="E38" s="84">
         <v>45467</v>
       </c>
+      <c r="F38" s="84">
+        <v>45467</v>
+      </c>
       <c r="M38" s="83">
         <v>545</v>
       </c>
@@ -19171,6 +19269,9 @@
       <c r="E39" s="84">
         <v>45468</v>
       </c>
+      <c r="F39" s="84">
+        <v>45468</v>
+      </c>
       <c r="M39" s="83">
         <v>545</v>
       </c>
@@ -19194,6 +19295,9 @@
       <c r="E40" s="84">
         <v>45470</v>
       </c>
+      <c r="F40" s="84">
+        <v>45470</v>
+      </c>
       <c r="M40" s="83">
         <v>545</v>
       </c>
@@ -19214,6 +19318,9 @@
       <c r="E41" s="84">
         <v>45474</v>
       </c>
+      <c r="F41" s="84">
+        <v>45474</v>
+      </c>
       <c r="M41" s="83">
         <v>515</v>
       </c>
@@ -19243,6 +19350,9 @@
       <c r="E42" s="84">
         <v>45488</v>
       </c>
+      <c r="F42" s="84">
+        <v>45488</v>
+      </c>
       <c r="M42" s="83">
         <v>401</v>
       </c>
@@ -19263,6 +19373,9 @@
       <c r="E43" s="84">
         <v>45492</v>
       </c>
+      <c r="F43" s="84">
+        <v>45492</v>
+      </c>
       <c r="M43" s="83">
         <v>481</v>
       </c>
@@ -19283,6 +19396,9 @@
       <c r="E44" s="84">
         <v>45498</v>
       </c>
+      <c r="F44" s="84">
+        <v>45498</v>
+      </c>
       <c r="M44" s="83">
         <v>556</v>
       </c>
@@ -19306,6 +19422,9 @@
       <c r="E45" s="84">
         <v>45518</v>
       </c>
+      <c r="F45" s="84">
+        <v>45518</v>
+      </c>
       <c r="M45" s="83">
         <v>146</v>
       </c>
@@ -19332,6 +19451,9 @@
       <c r="E46" s="84">
         <v>45524</v>
       </c>
+      <c r="F46" s="84">
+        <v>45524</v>
+      </c>
       <c r="O46" s="122" t="s">
         <v>1426</v>
       </c>
@@ -19349,6 +19471,9 @@
       <c r="E47" s="84">
         <v>45532</v>
       </c>
+      <c r="F47" s="84">
+        <v>45532</v>
+      </c>
       <c r="M47" s="83">
         <v>561</v>
       </c>
@@ -19381,6 +19506,9 @@
       <c r="E48" s="84">
         <v>45538</v>
       </c>
+      <c r="F48" s="84">
+        <v>45538</v>
+      </c>
       <c r="M48" s="83">
         <v>33</v>
       </c>
@@ -19404,6 +19532,9 @@
       <c r="E49" s="84">
         <v>45462</v>
       </c>
+      <c r="F49" s="84">
+        <v>45462</v>
+      </c>
       <c r="M49" s="83">
         <v>558</v>
       </c>
@@ -19453,6 +19584,9 @@
       <c r="E51" s="84">
         <v>45575</v>
       </c>
+      <c r="F51" s="84">
+        <v>45575</v>
+      </c>
       <c r="M51" s="83">
         <v>558</v>
       </c>
@@ -19479,6 +19613,9 @@
       <c r="E52" s="84">
         <v>45558</v>
       </c>
+      <c r="F52" s="84">
+        <v>45558</v>
+      </c>
       <c r="M52" s="83">
         <v>146</v>
       </c>
@@ -19505,6 +19642,9 @@
       <c r="E53" s="84">
         <v>45587</v>
       </c>
+      <c r="F53" s="84">
+        <v>45587</v>
+      </c>
       <c r="M53" s="83">
         <v>387</v>
       </c>
@@ -19528,6 +19668,9 @@
       <c r="E54" s="84">
         <v>45596</v>
       </c>
+      <c r="F54" s="84">
+        <v>45596</v>
+      </c>
       <c r="M54" s="83">
         <v>552</v>
       </c>
@@ -19554,6 +19697,9 @@
       <c r="E55" s="84">
         <v>45600</v>
       </c>
+      <c r="F55" s="84">
+        <v>45600</v>
+      </c>
       <c r="M55" s="83">
         <v>481</v>
       </c>
@@ -19580,6 +19726,9 @@
       <c r="E56" s="84">
         <v>45601</v>
       </c>
+      <c r="F56" s="84">
+        <v>45601</v>
+      </c>
       <c r="M56" s="83">
         <v>494</v>
       </c>
@@ -19603,6 +19752,9 @@
       <c r="E57" s="84">
         <v>45602</v>
       </c>
+      <c r="F57" s="84">
+        <v>45602</v>
+      </c>
       <c r="M57" s="83">
         <v>337</v>
       </c>
@@ -19629,6 +19781,9 @@
       <c r="E58" s="84">
         <v>45603</v>
       </c>
+      <c r="F58" s="84">
+        <v>45603</v>
+      </c>
       <c r="M58" s="83">
         <v>337</v>
       </c>
@@ -19655,6 +19810,9 @@
       <c r="E59" s="84">
         <v>45611</v>
       </c>
+      <c r="F59" s="84">
+        <v>45611</v>
+      </c>
       <c r="M59" s="83">
         <v>561</v>
       </c>
@@ -19684,6 +19842,9 @@
       <c r="E60" s="84">
         <v>45612</v>
       </c>
+      <c r="F60" s="84">
+        <v>45612</v>
+      </c>
       <c r="M60" s="83">
         <v>545</v>
       </c>
@@ -19707,6 +19868,9 @@
       <c r="E61" s="84">
         <v>45617</v>
       </c>
+      <c r="F61" s="84">
+        <v>45617</v>
+      </c>
       <c r="M61" s="83">
         <v>546</v>
       </c>
@@ -19730,6 +19894,9 @@
       <c r="E62" s="84">
         <v>45632</v>
       </c>
+      <c r="F62" s="84">
+        <v>45632</v>
+      </c>
       <c r="M62" s="83">
         <v>545</v>
       </c>
@@ -19762,6 +19929,9 @@
       <c r="E63" s="84">
         <v>45635</v>
       </c>
+      <c r="F63" s="84">
+        <v>45635</v>
+      </c>
       <c r="M63" s="83">
         <v>552</v>
       </c>
@@ -19791,6 +19961,9 @@
       <c r="E64" s="84">
         <v>45637</v>
       </c>
+      <c r="F64" s="84">
+        <v>45637</v>
+      </c>
       <c r="M64" s="83">
         <v>532</v>
       </c>
@@ -19817,6 +19990,9 @@
       <c r="E65" s="84">
         <v>45632</v>
       </c>
+      <c r="F65" s="84">
+        <v>45632</v>
+      </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66" s="83">
@@ -19831,6 +20007,9 @@
       <c r="E66" s="84">
         <v>45672</v>
       </c>
+      <c r="F66" s="84">
+        <v>45672</v>
+      </c>
       <c r="M66" s="83">
         <v>472</v>
       </c>
@@ -19854,6 +20033,9 @@
       <c r="E67" s="84">
         <v>45680</v>
       </c>
+      <c r="F67" s="84">
+        <v>45680</v>
+      </c>
       <c r="M67" s="83">
         <v>441</v>
       </c>
@@ -19886,6 +20068,9 @@
       <c r="E68" s="84">
         <v>45671</v>
       </c>
+      <c r="F68" s="84">
+        <v>45671</v>
+      </c>
       <c r="M68" s="83">
         <v>552</v>
       </c>
@@ -19916,7 +20101,7 @@
       <c r="E69" s="84">
         <v>45694</v>
       </c>
-      <c r="F69" s="125">
+      <c r="F69" s="84">
         <v>45694</v>
       </c>
       <c r="M69" s="83">
@@ -19948,6 +20133,9 @@
       <c r="E70" s="84">
         <v>45695</v>
       </c>
+      <c r="F70" s="84">
+        <v>45695</v>
+      </c>
       <c r="M70" s="83">
         <v>78</v>
       </c>
@@ -19971,6 +20159,9 @@
       <c r="E71" s="84">
         <v>45728</v>
       </c>
+      <c r="F71" s="84">
+        <v>45728</v>
+      </c>
       <c r="M71" s="83">
         <v>552</v>
       </c>
@@ -20000,6 +20191,9 @@
       <c r="E72" s="84">
         <v>45742</v>
       </c>
+      <c r="F72" s="84">
+        <v>45742</v>
+      </c>
       <c r="M72" s="83">
         <v>562</v>
       </c>
@@ -20023,6 +20217,9 @@
       <c r="E73" s="84">
         <v>45747</v>
       </c>
+      <c r="F73" s="84">
+        <v>45747</v>
+      </c>
       <c r="M73" s="83">
         <v>552</v>
       </c>
@@ -20052,6 +20249,9 @@
       <c r="E74" s="84">
         <v>45751</v>
       </c>
+      <c r="F74" s="84">
+        <v>45751</v>
+      </c>
       <c r="M74" s="83">
         <v>561</v>
       </c>
@@ -20084,6 +20284,9 @@
       <c r="E75" s="84">
         <v>45757</v>
       </c>
+      <c r="F75" s="84">
+        <v>45757</v>
+      </c>
       <c r="M75" s="83">
         <v>545</v>
       </c>
@@ -20116,6 +20319,9 @@
       <c r="E76" s="84">
         <v>45779</v>
       </c>
+      <c r="F76" s="84">
+        <v>45779</v>
+      </c>
       <c r="M76" s="83">
         <v>553</v>
       </c>
@@ -20148,13 +20354,16 @@
       <c r="E77" s="84">
         <v>45782</v>
       </c>
+      <c r="F77" s="84">
+        <v>45782</v>
+      </c>
       <c r="M77" s="83">
         <v>347</v>
       </c>
       <c r="N77" s="83" t="s">
         <v>1349</v>
       </c>
-      <c r="O77" s="126" t="s">
+      <c r="O77" s="125" t="s">
         <v>1479</v>
       </c>
     </row>
@@ -20206,6 +20415,9 @@
       <c r="E79" s="84">
         <v>45791</v>
       </c>
+      <c r="F79" s="84">
+        <v>45791</v>
+      </c>
       <c r="M79" s="83">
         <v>552</v>
       </c>
@@ -20226,10 +20438,13 @@
       <c r="C80" s="83">
         <v>739</v>
       </c>
-      <c r="D80" s="127" t="s">
+      <c r="D80" s="126" t="s">
         <v>1483</v>
       </c>
       <c r="E80" s="84">
+        <v>45838</v>
+      </c>
+      <c r="F80" s="84">
         <v>45838</v>
       </c>
       <c r="M80" s="83">
@@ -20258,10 +20473,13 @@
       <c r="C81" s="83">
         <v>740</v>
       </c>
-      <c r="D81" s="128" t="s">
+      <c r="D81" s="127" t="s">
         <v>1484</v>
       </c>
       <c r="E81" s="84">
+        <v>45838</v>
+      </c>
+      <c r="F81" s="84">
         <v>45838</v>
       </c>
       <c r="M81" s="83">
@@ -20328,6 +20546,9 @@
       <c r="E83" s="84">
         <v>45810</v>
       </c>
+      <c r="F83" s="84">
+        <v>45810</v>
+      </c>
       <c r="M83" s="83">
         <v>337</v>
       </c>
@@ -20351,6 +20572,9 @@
       <c r="E84" s="84">
         <v>45810</v>
       </c>
+      <c r="F84" s="84">
+        <v>45810</v>
+      </c>
       <c r="M84" s="83">
         <v>528</v>
       </c>
@@ -20374,6 +20598,9 @@
       <c r="E85" s="84">
         <v>45817</v>
       </c>
+      <c r="F85" s="84">
+        <v>45817</v>
+      </c>
       <c r="M85" s="1">
         <v>554</v>
       </c>
@@ -20397,13 +20624,16 @@
       <c r="E86" s="84">
         <v>45821</v>
       </c>
+      <c r="F86" s="84">
+        <v>45821</v>
+      </c>
       <c r="M86" s="83">
         <v>326</v>
       </c>
       <c r="N86" s="83" t="s">
         <v>1492</v>
       </c>
-      <c r="O86" s="129" t="s">
+      <c r="O86" s="128" t="s">
         <v>1493</v>
       </c>
       <c r="Q86" s="87" t="s">
@@ -20888,7 +21118,7 @@
       <c r="N105" s="83" t="s">
         <v>1346</v>
       </c>
-      <c r="O105" s="131" t="s">
+      <c r="O105" s="130" t="s">
         <v>1528</v>
       </c>
       <c r="Q105" s="87" t="s">
@@ -20949,20 +21179,20 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="R6:S6"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D1:T1"/>
     <mergeCell ref="D2:T2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:T3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="R6:S6"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7:F488">
+  <conditionalFormatting sqref="F12 F82 F87:F488">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>LEN(TRIM(F7))=0</formula>
+      <formula>LEN(TRIM(F12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>